<commit_message>
Correção do ranking principal
</commit_message>
<xml_diff>
--- a/src/resources/templates/ranking.xlsx
+++ b/src/resources/templates/ranking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\CopaLand\CopaLandWebApi\src\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8ADA83-CEB4-4987-9440-8809C30DA7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B26A246-A329-4D5B-A196-0F926AE611FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,9 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -398,7 +401,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,19 +439,19 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>